<commit_message>
add the missing file
</commit_message>
<xml_diff>
--- a/book_manual_inspections/per-book_chapters_labelling.xlsx
+++ b/book_manual_inspections/per-book_chapters_labelling.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="255">
   <si>
     <t>Agile Testing</t>
   </si>
@@ -1731,7 +1731,9 @@
       <c r="A4" s="2">
         <v>1.0</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" s="11"/>
       <c r="D4" s="4" t="s">
         <v>192</v>
@@ -3390,7 +3392,9 @@
       <c r="A12" s="8">
         <v>9.0</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C12" s="10"/>
       <c r="D12" s="9" t="s">
         <v>90</v>
@@ -3400,7 +3404,9 @@
       <c r="A13" s="8">
         <v>10.0</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
       <c r="C13" s="10"/>
       <c r="D13" s="9" t="s">
         <v>91</v>

</xml_diff>